<commit_message>
added ac remotes support
</commit_message>
<xml_diff>
--- a/ac translations/Danish.xlsx
+++ b/ac translations/Danish.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shabat\Desktop\example\new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\programming\Remote - Projects\helper projects\Remotes App Translation Project\ac translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Danish Translation" sheetId="1" r:id="rId1"/>
@@ -1210,9 +1210,6 @@
 Fjernbetjening til dit fjernsyn</t>
   </si>
   <si>
-    <t>Fjernbetjening til _____ - NU GRATIS</t>
-  </si>
-  <si>
     <t>Remote for ____ - NOW FREE</t>
   </si>
   <si>
@@ -1226,6 +1223,9 @@
   </si>
   <si>
     <t>GRATIS udgave i en begrænset periode</t>
+  </si>
+  <si>
+    <t>fuckkk</t>
   </si>
 </sst>
 </file>
@@ -1742,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="65" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1772,10 +1772,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -1783,16 +1783,16 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="F5" t="s">
         <v>387</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="F5" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>